<commit_message>
Updated to current version
</commit_message>
<xml_diff>
--- a/TopSky_Developer_Guide_Settings.xlsx
+++ b/TopSky_Developer_Guide_Settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juha\Documents\Office Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Documents\EuroScope\ENOR-Norway-NC-DEV\ENOR\Plugins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3CBB8F-B17B-4BDD-99A6-3E5932613E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12DEF7E-CC7F-440D-9855-A4964DA08C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15060" yWindow="5100" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TopSky 2.4" sheetId="1" r:id="rId1"/>
@@ -5583,7 +5583,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="330">
@@ -7667,7 +7667,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7990,14 +7990,14 @@
   <dimension ref="A1:K866"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="2" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B453" sqref="B453"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="137.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="5" customWidth="1"/>
     <col min="6" max="11" width="13.7109375" style="2" customWidth="1"/>
@@ -23421,7 +23421,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -24541,7 +24540,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
@@ -25431,7 +25430,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">

</xml_diff>